<commit_message>
Organization. Statistics. Recompiled for 4.0 Client Profile
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Pilots and trials/Pilot 6/Pilot 6 data.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Pilots and trials/Pilot 6/Pilot 6 data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="11">
   <si>
     <t>Participant Number</t>
   </si>
@@ -533,7 +533,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -880,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H145" sqref="A1:H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4656,6 +4658,3750 @@
       </c>
       <c r="H145" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="4">
+        <v>60</v>
+      </c>
+      <c r="B146" s="4">
+        <v>0</v>
+      </c>
+      <c r="C146" s="4">
+        <v>1</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="4">
+        <v>0</v>
+      </c>
+      <c r="F146" s="4">
+        <v>33090</v>
+      </c>
+      <c r="G146" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H146" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="4">
+        <v>60</v>
+      </c>
+      <c r="B147" s="4">
+        <v>1</v>
+      </c>
+      <c r="C147" s="4">
+        <v>1</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="4">
+        <v>0</v>
+      </c>
+      <c r="F147" s="4">
+        <v>12452</v>
+      </c>
+      <c r="G147" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H147" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="4">
+        <v>60</v>
+      </c>
+      <c r="B148" s="4">
+        <v>2</v>
+      </c>
+      <c r="C148" s="4">
+        <v>1</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" s="4">
+        <v>0</v>
+      </c>
+      <c r="F148" s="4">
+        <v>28198</v>
+      </c>
+      <c r="G148" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H148" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="4">
+        <v>60</v>
+      </c>
+      <c r="B149" s="4">
+        <v>3</v>
+      </c>
+      <c r="C149" s="4">
+        <v>1</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0</v>
+      </c>
+      <c r="F149" s="4">
+        <v>18236</v>
+      </c>
+      <c r="G149" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H149" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="4">
+        <v>60</v>
+      </c>
+      <c r="B150" s="4">
+        <v>4</v>
+      </c>
+      <c r="C150" s="4">
+        <v>1</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="4">
+        <v>1</v>
+      </c>
+      <c r="F150" s="4">
+        <v>15140</v>
+      </c>
+      <c r="G150" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H150" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <v>60</v>
+      </c>
+      <c r="B151" s="4">
+        <v>5</v>
+      </c>
+      <c r="C151" s="4">
+        <v>1</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="4">
+        <v>1</v>
+      </c>
+      <c r="F151" s="4">
+        <v>11428</v>
+      </c>
+      <c r="G151" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H151" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="4">
+        <v>60</v>
+      </c>
+      <c r="B152" s="4">
+        <v>6</v>
+      </c>
+      <c r="C152" s="4">
+        <v>1</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="4">
+        <v>1</v>
+      </c>
+      <c r="F152" s="4">
+        <v>20772</v>
+      </c>
+      <c r="G152" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H152" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="4">
+        <v>60</v>
+      </c>
+      <c r="B153" s="4">
+        <v>7</v>
+      </c>
+      <c r="C153" s="4">
+        <v>1</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" s="4">
+        <v>1</v>
+      </c>
+      <c r="F153" s="4">
+        <v>45236</v>
+      </c>
+      <c r="G153" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H153" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="4">
+        <v>60</v>
+      </c>
+      <c r="B154" s="4">
+        <v>8</v>
+      </c>
+      <c r="C154" s="4">
+        <v>1</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" s="4">
+        <v>0</v>
+      </c>
+      <c r="F154" s="4">
+        <v>25363</v>
+      </c>
+      <c r="G154" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H154" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="4">
+        <v>60</v>
+      </c>
+      <c r="B155" s="4">
+        <v>9</v>
+      </c>
+      <c r="C155" s="4">
+        <v>1</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" s="4">
+        <v>0</v>
+      </c>
+      <c r="F155" s="4">
+        <v>54432</v>
+      </c>
+      <c r="G155" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H155" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="4">
+        <v>60</v>
+      </c>
+      <c r="B156" s="4">
+        <v>10</v>
+      </c>
+      <c r="C156" s="4">
+        <v>1</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="4">
+        <v>0</v>
+      </c>
+      <c r="F156" s="4">
+        <v>16417</v>
+      </c>
+      <c r="G156" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H156" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="4">
+        <v>60</v>
+      </c>
+      <c r="B157" s="4">
+        <v>11</v>
+      </c>
+      <c r="C157" s="4">
+        <v>1</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="4">
+        <v>0</v>
+      </c>
+      <c r="F157" s="4">
+        <v>25488</v>
+      </c>
+      <c r="G157" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H157" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="4">
+        <v>60</v>
+      </c>
+      <c r="B158" s="4">
+        <v>12</v>
+      </c>
+      <c r="C158" s="4">
+        <v>1</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" s="4">
+        <v>1</v>
+      </c>
+      <c r="F158" s="4">
+        <v>14041</v>
+      </c>
+      <c r="G158" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H158" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="4">
+        <v>60</v>
+      </c>
+      <c r="B159" s="4">
+        <v>13</v>
+      </c>
+      <c r="C159" s="4">
+        <v>1</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="4">
+        <v>1</v>
+      </c>
+      <c r="F159" s="4">
+        <v>23490</v>
+      </c>
+      <c r="G159" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H159" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="4">
+        <v>60</v>
+      </c>
+      <c r="B160" s="4">
+        <v>14</v>
+      </c>
+      <c r="C160" s="4">
+        <v>1</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" s="4">
+        <v>1</v>
+      </c>
+      <c r="F160" s="4">
+        <v>24225</v>
+      </c>
+      <c r="G160" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H160" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="4">
+        <v>60</v>
+      </c>
+      <c r="B161" s="4">
+        <v>15</v>
+      </c>
+      <c r="C161" s="4">
+        <v>1</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" s="4">
+        <v>1</v>
+      </c>
+      <c r="F161" s="4">
+        <v>21881</v>
+      </c>
+      <c r="G161" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H161" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="4">
+        <v>60</v>
+      </c>
+      <c r="B162" s="4">
+        <v>16</v>
+      </c>
+      <c r="C162" s="4">
+        <v>2</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" s="4">
+        <v>0</v>
+      </c>
+      <c r="F162" s="4">
+        <v>36524</v>
+      </c>
+      <c r="G162" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H162" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="4">
+        <v>60</v>
+      </c>
+      <c r="B163" s="4">
+        <v>17</v>
+      </c>
+      <c r="C163" s="4">
+        <v>2</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E163" s="4">
+        <v>0</v>
+      </c>
+      <c r="F163" s="4">
+        <v>31716</v>
+      </c>
+      <c r="G163" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H163" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="4">
+        <v>60</v>
+      </c>
+      <c r="B164" s="4">
+        <v>18</v>
+      </c>
+      <c r="C164" s="4">
+        <v>2</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E164" s="4">
+        <v>0</v>
+      </c>
+      <c r="F164" s="4">
+        <v>15563</v>
+      </c>
+      <c r="G164" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H164" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="4">
+        <v>60</v>
+      </c>
+      <c r="B165" s="4">
+        <v>19</v>
+      </c>
+      <c r="C165" s="4">
+        <v>2</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E165" s="4">
+        <v>0</v>
+      </c>
+      <c r="F165" s="4">
+        <v>18844</v>
+      </c>
+      <c r="G165" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H165" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="4">
+        <v>60</v>
+      </c>
+      <c r="B166" s="4">
+        <v>20</v>
+      </c>
+      <c r="C166" s="4">
+        <v>2</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="4">
+        <v>1</v>
+      </c>
+      <c r="F166" s="4">
+        <v>16348</v>
+      </c>
+      <c r="G166" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H166" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="4">
+        <v>60</v>
+      </c>
+      <c r="B167" s="4">
+        <v>21</v>
+      </c>
+      <c r="C167" s="4">
+        <v>2</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E167" s="4">
+        <v>1</v>
+      </c>
+      <c r="F167" s="4">
+        <v>9980</v>
+      </c>
+      <c r="G167" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H167" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="4">
+        <v>60</v>
+      </c>
+      <c r="B168" s="4">
+        <v>22</v>
+      </c>
+      <c r="C168" s="4">
+        <v>2</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" s="4">
+        <v>1</v>
+      </c>
+      <c r="F168" s="4">
+        <v>17108</v>
+      </c>
+      <c r="G168" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H168" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="4">
+        <v>60</v>
+      </c>
+      <c r="B169" s="4">
+        <v>23</v>
+      </c>
+      <c r="C169" s="4">
+        <v>2</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" s="4">
+        <v>1</v>
+      </c>
+      <c r="F169" s="4">
+        <v>39891</v>
+      </c>
+      <c r="G169" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H169" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="4">
+        <v>60</v>
+      </c>
+      <c r="B170" s="4">
+        <v>24</v>
+      </c>
+      <c r="C170" s="4">
+        <v>2</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E170" s="4">
+        <v>0</v>
+      </c>
+      <c r="F170" s="4">
+        <v>22241</v>
+      </c>
+      <c r="G170" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H170" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="4">
+        <v>60</v>
+      </c>
+      <c r="B171" s="4">
+        <v>25</v>
+      </c>
+      <c r="C171" s="4">
+        <v>2</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E171" s="4">
+        <v>0</v>
+      </c>
+      <c r="F171" s="4">
+        <v>47193</v>
+      </c>
+      <c r="G171" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H171" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="4">
+        <v>60</v>
+      </c>
+      <c r="B172" s="4">
+        <v>26</v>
+      </c>
+      <c r="C172" s="4">
+        <v>2</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E172" s="4">
+        <v>0</v>
+      </c>
+      <c r="F172" s="4">
+        <v>13616</v>
+      </c>
+      <c r="G172" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H172" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="4">
+        <v>60</v>
+      </c>
+      <c r="B173" s="4">
+        <v>27</v>
+      </c>
+      <c r="C173" s="4">
+        <v>2</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E173" s="4">
+        <v>0</v>
+      </c>
+      <c r="F173" s="4">
+        <v>15664</v>
+      </c>
+      <c r="G173" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H173" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="4">
+        <v>60</v>
+      </c>
+      <c r="B174" s="4">
+        <v>28</v>
+      </c>
+      <c r="C174" s="4">
+        <v>2</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" s="4">
+        <v>1</v>
+      </c>
+      <c r="F174" s="4">
+        <v>14092</v>
+      </c>
+      <c r="G174" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H174" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="4">
+        <v>60</v>
+      </c>
+      <c r="B175" s="4">
+        <v>29</v>
+      </c>
+      <c r="C175" s="4">
+        <v>2</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" s="4">
+        <v>1</v>
+      </c>
+      <c r="F175" s="4">
+        <v>14673</v>
+      </c>
+      <c r="G175" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H175" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="4">
+        <v>60</v>
+      </c>
+      <c r="B176" s="4">
+        <v>30</v>
+      </c>
+      <c r="C176" s="4">
+        <v>2</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="4">
+        <v>1</v>
+      </c>
+      <c r="F176" s="4">
+        <v>4601</v>
+      </c>
+      <c r="G176" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H176" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="4">
+        <v>60</v>
+      </c>
+      <c r="B177" s="4">
+        <v>31</v>
+      </c>
+      <c r="C177" s="4">
+        <v>2</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E177" s="4">
+        <v>1</v>
+      </c>
+      <c r="F177" s="4">
+        <v>16274</v>
+      </c>
+      <c r="G177" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H177" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="4">
+        <v>60</v>
+      </c>
+      <c r="B178" s="4">
+        <v>32</v>
+      </c>
+      <c r="C178" s="4">
+        <v>0</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="4">
+        <v>0</v>
+      </c>
+      <c r="F178" s="4">
+        <v>30397</v>
+      </c>
+      <c r="G178" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H178" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="4">
+        <v>60</v>
+      </c>
+      <c r="B179" s="4">
+        <v>33</v>
+      </c>
+      <c r="C179" s="4">
+        <v>0</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" s="4">
+        <v>0</v>
+      </c>
+      <c r="F179" s="4">
+        <v>14853</v>
+      </c>
+      <c r="G179" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H179" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="4">
+        <v>60</v>
+      </c>
+      <c r="B180" s="4">
+        <v>34</v>
+      </c>
+      <c r="C180" s="4">
+        <v>0</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" s="4">
+        <v>0</v>
+      </c>
+      <c r="F180" s="4">
+        <v>15949</v>
+      </c>
+      <c r="G180" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H180" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="4">
+        <v>60</v>
+      </c>
+      <c r="B181" s="4">
+        <v>35</v>
+      </c>
+      <c r="C181" s="4">
+        <v>0</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E181" s="4">
+        <v>0</v>
+      </c>
+      <c r="F181" s="4">
+        <v>20228</v>
+      </c>
+      <c r="G181" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H181" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="4">
+        <v>60</v>
+      </c>
+      <c r="B182" s="4">
+        <v>36</v>
+      </c>
+      <c r="C182" s="4">
+        <v>0</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" s="4">
+        <v>1</v>
+      </c>
+      <c r="F182" s="4">
+        <v>29932</v>
+      </c>
+      <c r="G182" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H182" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="4">
+        <v>60</v>
+      </c>
+      <c r="B183" s="4">
+        <v>37</v>
+      </c>
+      <c r="C183" s="4">
+        <v>0</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="4">
+        <v>1</v>
+      </c>
+      <c r="F183" s="4">
+        <v>13116</v>
+      </c>
+      <c r="G183" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H183" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="4">
+        <v>60</v>
+      </c>
+      <c r="B184" s="4">
+        <v>38</v>
+      </c>
+      <c r="C184" s="4">
+        <v>0</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" s="4">
+        <v>1</v>
+      </c>
+      <c r="F184" s="4">
+        <v>29124</v>
+      </c>
+      <c r="G184" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H184" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="4">
+        <v>60</v>
+      </c>
+      <c r="B185" s="4">
+        <v>39</v>
+      </c>
+      <c r="C185" s="4">
+        <v>0</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="4">
+        <v>1</v>
+      </c>
+      <c r="F185" s="4">
+        <v>14324</v>
+      </c>
+      <c r="G185" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H185" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="4">
+        <v>60</v>
+      </c>
+      <c r="B186" s="4">
+        <v>40</v>
+      </c>
+      <c r="C186" s="4">
+        <v>0</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E186" s="4">
+        <v>0</v>
+      </c>
+      <c r="F186" s="4">
+        <v>21112</v>
+      </c>
+      <c r="G186" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H186" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="4">
+        <v>60</v>
+      </c>
+      <c r="B187" s="4">
+        <v>41</v>
+      </c>
+      <c r="C187" s="4">
+        <v>0</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E187" s="4">
+        <v>0</v>
+      </c>
+      <c r="F187" s="4">
+        <v>44800</v>
+      </c>
+      <c r="G187" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H187" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="4">
+        <v>60</v>
+      </c>
+      <c r="B188" s="4">
+        <v>42</v>
+      </c>
+      <c r="C188" s="4">
+        <v>0</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E188" s="4">
+        <v>0</v>
+      </c>
+      <c r="F188" s="4">
+        <v>12441</v>
+      </c>
+      <c r="G188" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H188" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="4">
+        <v>60</v>
+      </c>
+      <c r="B189" s="4">
+        <v>43</v>
+      </c>
+      <c r="C189" s="4">
+        <v>0</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E189" s="4">
+        <v>0</v>
+      </c>
+      <c r="F189" s="4">
+        <v>35770</v>
+      </c>
+      <c r="G189" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H189" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="4">
+        <v>60</v>
+      </c>
+      <c r="B190" s="4">
+        <v>44</v>
+      </c>
+      <c r="C190" s="4">
+        <v>0</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E190" s="4">
+        <v>1</v>
+      </c>
+      <c r="F190" s="4">
+        <v>37752</v>
+      </c>
+      <c r="G190" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H190" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="4">
+        <v>60</v>
+      </c>
+      <c r="B191" s="4">
+        <v>45</v>
+      </c>
+      <c r="C191" s="4">
+        <v>0</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191" s="4">
+        <v>1</v>
+      </c>
+      <c r="F191" s="4">
+        <v>14874</v>
+      </c>
+      <c r="G191" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H191" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="4">
+        <v>60</v>
+      </c>
+      <c r="B192" s="4">
+        <v>46</v>
+      </c>
+      <c r="C192" s="4">
+        <v>0</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" s="4">
+        <v>1</v>
+      </c>
+      <c r="F192" s="4">
+        <v>12848</v>
+      </c>
+      <c r="G192" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H192" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="4">
+        <v>60</v>
+      </c>
+      <c r="B193" s="4">
+        <v>47</v>
+      </c>
+      <c r="C193" s="4">
+        <v>0</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E193" s="4">
+        <v>1</v>
+      </c>
+      <c r="F193" s="4">
+        <v>34848</v>
+      </c>
+      <c r="G193" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H193" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" s="5">
+        <v>61</v>
+      </c>
+      <c r="B194" s="5">
+        <v>0</v>
+      </c>
+      <c r="C194" s="5">
+        <v>0</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E194" s="5">
+        <v>0</v>
+      </c>
+      <c r="F194" s="5">
+        <v>30615</v>
+      </c>
+      <c r="G194" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H194" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="5">
+        <v>61</v>
+      </c>
+      <c r="B195" s="5">
+        <v>1</v>
+      </c>
+      <c r="C195" s="5">
+        <v>0</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E195" s="5">
+        <v>0</v>
+      </c>
+      <c r="F195" s="5">
+        <v>68129</v>
+      </c>
+      <c r="G195" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H195" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" s="5">
+        <v>61</v>
+      </c>
+      <c r="B196" s="5">
+        <v>2</v>
+      </c>
+      <c r="C196" s="5">
+        <v>0</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E196" s="5">
+        <v>0</v>
+      </c>
+      <c r="F196" s="5">
+        <v>18457</v>
+      </c>
+      <c r="G196" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H196" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="5">
+        <v>61</v>
+      </c>
+      <c r="B197" s="5">
+        <v>3</v>
+      </c>
+      <c r="C197" s="5">
+        <v>0</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E197" s="5">
+        <v>0</v>
+      </c>
+      <c r="F197" s="5">
+        <v>21378</v>
+      </c>
+      <c r="G197" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H197" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="5">
+        <v>61</v>
+      </c>
+      <c r="B198" s="5">
+        <v>4</v>
+      </c>
+      <c r="C198" s="5">
+        <v>0</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E198" s="5">
+        <v>1</v>
+      </c>
+      <c r="F198" s="5">
+        <v>38492</v>
+      </c>
+      <c r="G198" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H198" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="5">
+        <v>61</v>
+      </c>
+      <c r="B199" s="5">
+        <v>5</v>
+      </c>
+      <c r="C199" s="5">
+        <v>0</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E199" s="5">
+        <v>1</v>
+      </c>
+      <c r="F199" s="5">
+        <v>22386</v>
+      </c>
+      <c r="G199" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H199" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="5">
+        <v>61</v>
+      </c>
+      <c r="B200" s="5">
+        <v>6</v>
+      </c>
+      <c r="C200" s="5">
+        <v>0</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" s="5">
+        <v>1</v>
+      </c>
+      <c r="F200" s="5">
+        <v>25844</v>
+      </c>
+      <c r="G200" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H200" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="5">
+        <v>61</v>
+      </c>
+      <c r="B201" s="5">
+        <v>7</v>
+      </c>
+      <c r="C201" s="5">
+        <v>0</v>
+      </c>
+      <c r="D201" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" s="5">
+        <v>1</v>
+      </c>
+      <c r="F201" s="5">
+        <v>24112</v>
+      </c>
+      <c r="G201" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H201" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="5">
+        <v>61</v>
+      </c>
+      <c r="B202" s="5">
+        <v>8</v>
+      </c>
+      <c r="C202" s="5">
+        <v>0</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E202" s="5">
+        <v>0</v>
+      </c>
+      <c r="F202" s="5">
+        <v>31272</v>
+      </c>
+      <c r="G202" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H202" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="5">
+        <v>61</v>
+      </c>
+      <c r="B203" s="5">
+        <v>9</v>
+      </c>
+      <c r="C203" s="5">
+        <v>0</v>
+      </c>
+      <c r="D203" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" s="5">
+        <v>0</v>
+      </c>
+      <c r="F203" s="5">
+        <v>19316</v>
+      </c>
+      <c r="G203" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H203" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="5">
+        <v>61</v>
+      </c>
+      <c r="B204" s="5">
+        <v>10</v>
+      </c>
+      <c r="C204" s="5">
+        <v>0</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" s="5">
+        <v>0</v>
+      </c>
+      <c r="F204" s="5">
+        <v>20148</v>
+      </c>
+      <c r="G204" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H204" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="5">
+        <v>61</v>
+      </c>
+      <c r="B205" s="5">
+        <v>11</v>
+      </c>
+      <c r="C205" s="5">
+        <v>0</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" s="5">
+        <v>0</v>
+      </c>
+      <c r="F205" s="5">
+        <v>21084</v>
+      </c>
+      <c r="G205" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H205" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="5">
+        <v>61</v>
+      </c>
+      <c r="B206" s="5">
+        <v>12</v>
+      </c>
+      <c r="C206" s="5">
+        <v>0</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E206" s="5">
+        <v>1</v>
+      </c>
+      <c r="F206" s="5">
+        <v>14036</v>
+      </c>
+      <c r="G206" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H206" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="5">
+        <v>61</v>
+      </c>
+      <c r="B207" s="5">
+        <v>13</v>
+      </c>
+      <c r="C207" s="5">
+        <v>0</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E207" s="5">
+        <v>1</v>
+      </c>
+      <c r="F207" s="5">
+        <v>16012</v>
+      </c>
+      <c r="G207" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H207" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="5">
+        <v>61</v>
+      </c>
+      <c r="B208" s="5">
+        <v>14</v>
+      </c>
+      <c r="C208" s="5">
+        <v>0</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E208" s="5">
+        <v>1</v>
+      </c>
+      <c r="F208" s="5">
+        <v>8341</v>
+      </c>
+      <c r="G208" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H208" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="5">
+        <v>61</v>
+      </c>
+      <c r="B209" s="5">
+        <v>15</v>
+      </c>
+      <c r="C209" s="5">
+        <v>0</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E209" s="5">
+        <v>1</v>
+      </c>
+      <c r="F209" s="5">
+        <v>14045</v>
+      </c>
+      <c r="G209" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H209" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="5">
+        <v>61</v>
+      </c>
+      <c r="B210" s="5">
+        <v>16</v>
+      </c>
+      <c r="C210" s="5">
+        <v>2</v>
+      </c>
+      <c r="D210" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E210" s="5">
+        <v>0</v>
+      </c>
+      <c r="F210" s="5">
+        <v>19426</v>
+      </c>
+      <c r="G210" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H210" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="5">
+        <v>61</v>
+      </c>
+      <c r="B211" s="5">
+        <v>17</v>
+      </c>
+      <c r="C211" s="5">
+        <v>2</v>
+      </c>
+      <c r="D211" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E211" s="5">
+        <v>0</v>
+      </c>
+      <c r="F211" s="5">
+        <v>18825</v>
+      </c>
+      <c r="G211" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H211" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" s="5">
+        <v>61</v>
+      </c>
+      <c r="B212" s="5">
+        <v>18</v>
+      </c>
+      <c r="C212" s="5">
+        <v>2</v>
+      </c>
+      <c r="D212" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E212" s="5">
+        <v>0</v>
+      </c>
+      <c r="F212" s="5">
+        <v>36536</v>
+      </c>
+      <c r="G212" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H212" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="5">
+        <v>61</v>
+      </c>
+      <c r="B213" s="5">
+        <v>19</v>
+      </c>
+      <c r="C213" s="5">
+        <v>2</v>
+      </c>
+      <c r="D213" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E213" s="5">
+        <v>0</v>
+      </c>
+      <c r="F213" s="5">
+        <v>18370</v>
+      </c>
+      <c r="G213" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H213" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" s="5">
+        <v>61</v>
+      </c>
+      <c r="B214" s="5">
+        <v>20</v>
+      </c>
+      <c r="C214" s="5">
+        <v>2</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E214" s="5">
+        <v>1</v>
+      </c>
+      <c r="F214" s="5">
+        <v>28568</v>
+      </c>
+      <c r="G214" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H214" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A215" s="5">
+        <v>61</v>
+      </c>
+      <c r="B215" s="5">
+        <v>21</v>
+      </c>
+      <c r="C215" s="5">
+        <v>2</v>
+      </c>
+      <c r="D215" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E215" s="5">
+        <v>1</v>
+      </c>
+      <c r="F215" s="5">
+        <v>22009</v>
+      </c>
+      <c r="G215" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H215" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A216" s="5">
+        <v>61</v>
+      </c>
+      <c r="B216" s="5">
+        <v>22</v>
+      </c>
+      <c r="C216" s="5">
+        <v>2</v>
+      </c>
+      <c r="D216" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E216" s="5">
+        <v>1</v>
+      </c>
+      <c r="F216" s="5">
+        <v>15841</v>
+      </c>
+      <c r="G216" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H216" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A217" s="5">
+        <v>61</v>
+      </c>
+      <c r="B217" s="5">
+        <v>23</v>
+      </c>
+      <c r="C217" s="5">
+        <v>2</v>
+      </c>
+      <c r="D217" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E217" s="5">
+        <v>1</v>
+      </c>
+      <c r="F217" s="5">
+        <v>24568</v>
+      </c>
+      <c r="G217" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H217" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A218" s="5">
+        <v>61</v>
+      </c>
+      <c r="B218" s="5">
+        <v>24</v>
+      </c>
+      <c r="C218" s="5">
+        <v>2</v>
+      </c>
+      <c r="D218" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E218" s="5">
+        <v>0</v>
+      </c>
+      <c r="F218" s="5">
+        <v>43508</v>
+      </c>
+      <c r="G218" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H218" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A219" s="5">
+        <v>61</v>
+      </c>
+      <c r="B219" s="5">
+        <v>25</v>
+      </c>
+      <c r="C219" s="5">
+        <v>2</v>
+      </c>
+      <c r="D219" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E219" s="5">
+        <v>0</v>
+      </c>
+      <c r="F219" s="5">
+        <v>19492</v>
+      </c>
+      <c r="G219" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H219" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" s="5">
+        <v>61</v>
+      </c>
+      <c r="B220" s="5">
+        <v>26</v>
+      </c>
+      <c r="C220" s="5">
+        <v>2</v>
+      </c>
+      <c r="D220" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" s="5">
+        <v>0</v>
+      </c>
+      <c r="F220" s="5">
+        <v>25498</v>
+      </c>
+      <c r="G220" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H220" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="5">
+        <v>61</v>
+      </c>
+      <c r="B221" s="5">
+        <v>27</v>
+      </c>
+      <c r="C221" s="5">
+        <v>2</v>
+      </c>
+      <c r="D221" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E221" s="5">
+        <v>0</v>
+      </c>
+      <c r="F221" s="5">
+        <v>13573</v>
+      </c>
+      <c r="G221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H221" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="5">
+        <v>61</v>
+      </c>
+      <c r="B222" s="5">
+        <v>28</v>
+      </c>
+      <c r="C222" s="5">
+        <v>2</v>
+      </c>
+      <c r="D222" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E222" s="5">
+        <v>1</v>
+      </c>
+      <c r="F222" s="5">
+        <v>14708</v>
+      </c>
+      <c r="G222" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H222" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="5">
+        <v>61</v>
+      </c>
+      <c r="B223" s="5">
+        <v>29</v>
+      </c>
+      <c r="C223" s="5">
+        <v>2</v>
+      </c>
+      <c r="D223" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E223" s="5">
+        <v>1</v>
+      </c>
+      <c r="F223" s="5">
+        <v>18716</v>
+      </c>
+      <c r="G223" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H223" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224" s="5">
+        <v>61</v>
+      </c>
+      <c r="B224" s="5">
+        <v>30</v>
+      </c>
+      <c r="C224" s="5">
+        <v>2</v>
+      </c>
+      <c r="D224" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E224" s="5">
+        <v>1</v>
+      </c>
+      <c r="F224" s="5">
+        <v>14196</v>
+      </c>
+      <c r="G224" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H224" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="5">
+        <v>61</v>
+      </c>
+      <c r="B225" s="5">
+        <v>31</v>
+      </c>
+      <c r="C225" s="5">
+        <v>2</v>
+      </c>
+      <c r="D225" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E225" s="5">
+        <v>1</v>
+      </c>
+      <c r="F225" s="5">
+        <v>29348</v>
+      </c>
+      <c r="G225" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H225" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="5">
+        <v>61</v>
+      </c>
+      <c r="B226" s="5">
+        <v>32</v>
+      </c>
+      <c r="C226" s="5">
+        <v>1</v>
+      </c>
+      <c r="D226" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E226" s="5">
+        <v>0</v>
+      </c>
+      <c r="F226" s="5">
+        <v>17033</v>
+      </c>
+      <c r="G226" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H226" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" s="5">
+        <v>61</v>
+      </c>
+      <c r="B227" s="5">
+        <v>33</v>
+      </c>
+      <c r="C227" s="5">
+        <v>1</v>
+      </c>
+      <c r="D227" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E227" s="5">
+        <v>0</v>
+      </c>
+      <c r="F227" s="5">
+        <v>41416</v>
+      </c>
+      <c r="G227" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H227" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A228" s="5">
+        <v>61</v>
+      </c>
+      <c r="B228" s="5">
+        <v>34</v>
+      </c>
+      <c r="C228" s="5">
+        <v>1</v>
+      </c>
+      <c r="D228" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E228" s="5">
+        <v>0</v>
+      </c>
+      <c r="F228" s="5">
+        <v>19873</v>
+      </c>
+      <c r="G228" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H228" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="5">
+        <v>61</v>
+      </c>
+      <c r="B229" s="5">
+        <v>35</v>
+      </c>
+      <c r="C229" s="5">
+        <v>1</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E229" s="5">
+        <v>0</v>
+      </c>
+      <c r="F229" s="5">
+        <v>29801</v>
+      </c>
+      <c r="G229" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H229" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A230" s="5">
+        <v>61</v>
+      </c>
+      <c r="B230" s="5">
+        <v>36</v>
+      </c>
+      <c r="C230" s="5">
+        <v>1</v>
+      </c>
+      <c r="D230" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E230" s="5">
+        <v>1</v>
+      </c>
+      <c r="F230" s="5">
+        <v>44985</v>
+      </c>
+      <c r="G230" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H230" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A231" s="5">
+        <v>61</v>
+      </c>
+      <c r="B231" s="5">
+        <v>37</v>
+      </c>
+      <c r="C231" s="5">
+        <v>1</v>
+      </c>
+      <c r="D231" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E231" s="5">
+        <v>1</v>
+      </c>
+      <c r="F231" s="5">
+        <v>38768</v>
+      </c>
+      <c r="G231" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H231" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="5">
+        <v>61</v>
+      </c>
+      <c r="B232" s="5">
+        <v>38</v>
+      </c>
+      <c r="C232" s="5">
+        <v>1</v>
+      </c>
+      <c r="D232" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E232" s="5">
+        <v>1</v>
+      </c>
+      <c r="F232" s="5">
+        <v>21953</v>
+      </c>
+      <c r="G232" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H232" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" s="5">
+        <v>61</v>
+      </c>
+      <c r="B233" s="5">
+        <v>39</v>
+      </c>
+      <c r="C233" s="5">
+        <v>1</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E233" s="5">
+        <v>1</v>
+      </c>
+      <c r="F233" s="5">
+        <v>18505</v>
+      </c>
+      <c r="G233" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H233" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" s="5">
+        <v>61</v>
+      </c>
+      <c r="B234" s="5">
+        <v>40</v>
+      </c>
+      <c r="C234" s="5">
+        <v>1</v>
+      </c>
+      <c r="D234" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E234" s="5">
+        <v>0</v>
+      </c>
+      <c r="F234" s="5">
+        <v>39301</v>
+      </c>
+      <c r="G234" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H234" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" s="5">
+        <v>61</v>
+      </c>
+      <c r="B235" s="5">
+        <v>41</v>
+      </c>
+      <c r="C235" s="5">
+        <v>1</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" s="5">
+        <v>0</v>
+      </c>
+      <c r="F235" s="5">
+        <v>45116</v>
+      </c>
+      <c r="G235" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H235" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" s="5">
+        <v>61</v>
+      </c>
+      <c r="B236" s="5">
+        <v>42</v>
+      </c>
+      <c r="C236" s="5">
+        <v>1</v>
+      </c>
+      <c r="D236" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E236" s="5">
+        <v>0</v>
+      </c>
+      <c r="F236" s="5">
+        <v>11660</v>
+      </c>
+      <c r="G236" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H236" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" s="5">
+        <v>61</v>
+      </c>
+      <c r="B237" s="5">
+        <v>43</v>
+      </c>
+      <c r="C237" s="5">
+        <v>1</v>
+      </c>
+      <c r="D237" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E237" s="5">
+        <v>0</v>
+      </c>
+      <c r="F237" s="5">
+        <v>16828</v>
+      </c>
+      <c r="G237" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H237" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="5">
+        <v>61</v>
+      </c>
+      <c r="B238" s="5">
+        <v>44</v>
+      </c>
+      <c r="C238" s="5">
+        <v>1</v>
+      </c>
+      <c r="D238" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E238" s="5">
+        <v>1</v>
+      </c>
+      <c r="F238" s="5">
+        <v>19996</v>
+      </c>
+      <c r="G238" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H238" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="5">
+        <v>61</v>
+      </c>
+      <c r="B239" s="5">
+        <v>45</v>
+      </c>
+      <c r="C239" s="5">
+        <v>1</v>
+      </c>
+      <c r="D239" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E239" s="5">
+        <v>1</v>
+      </c>
+      <c r="F239" s="5">
+        <v>25004</v>
+      </c>
+      <c r="G239" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H239" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="5">
+        <v>61</v>
+      </c>
+      <c r="B240" s="5">
+        <v>46</v>
+      </c>
+      <c r="C240" s="5">
+        <v>1</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240" s="5">
+        <v>1</v>
+      </c>
+      <c r="F240" s="5">
+        <v>28844</v>
+      </c>
+      <c r="G240" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H240" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241" s="5">
+        <v>61</v>
+      </c>
+      <c r="B241" s="5">
+        <v>47</v>
+      </c>
+      <c r="C241" s="5">
+        <v>1</v>
+      </c>
+      <c r="D241" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E241" s="5">
+        <v>1</v>
+      </c>
+      <c r="F241" s="5">
+        <v>27788</v>
+      </c>
+      <c r="G241" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H241" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242" s="5">
+        <v>62</v>
+      </c>
+      <c r="B242" s="5">
+        <v>0</v>
+      </c>
+      <c r="C242" s="5">
+        <v>1</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E242" s="5">
+        <v>0</v>
+      </c>
+      <c r="F242" s="5">
+        <v>73645</v>
+      </c>
+      <c r="G242" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H242" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A243" s="5">
+        <v>62</v>
+      </c>
+      <c r="B243" s="5">
+        <v>1</v>
+      </c>
+      <c r="C243" s="5">
+        <v>1</v>
+      </c>
+      <c r="D243" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E243" s="5">
+        <v>0</v>
+      </c>
+      <c r="F243" s="5">
+        <v>14721</v>
+      </c>
+      <c r="G243" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H243" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A244" s="5">
+        <v>62</v>
+      </c>
+      <c r="B244" s="5">
+        <v>2</v>
+      </c>
+      <c r="C244" s="5">
+        <v>1</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E244" s="5">
+        <v>0</v>
+      </c>
+      <c r="F244" s="5">
+        <v>21499</v>
+      </c>
+      <c r="G244" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H244" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245" s="5">
+        <v>62</v>
+      </c>
+      <c r="B245" s="5">
+        <v>3</v>
+      </c>
+      <c r="C245" s="5">
+        <v>1</v>
+      </c>
+      <c r="D245" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E245" s="5">
+        <v>0</v>
+      </c>
+      <c r="F245" s="5">
+        <v>18712</v>
+      </c>
+      <c r="G245" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H245" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" s="5">
+        <v>62</v>
+      </c>
+      <c r="B246" s="5">
+        <v>4</v>
+      </c>
+      <c r="C246" s="5">
+        <v>1</v>
+      </c>
+      <c r="D246" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E246" s="5">
+        <v>1</v>
+      </c>
+      <c r="F246" s="5">
+        <v>54128</v>
+      </c>
+      <c r="G246" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H246" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A247" s="5">
+        <v>62</v>
+      </c>
+      <c r="B247" s="5">
+        <v>5</v>
+      </c>
+      <c r="C247" s="5">
+        <v>1</v>
+      </c>
+      <c r="D247" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E247" s="5">
+        <v>1</v>
+      </c>
+      <c r="F247" s="5">
+        <v>28393</v>
+      </c>
+      <c r="G247" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H247" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A248" s="5">
+        <v>62</v>
+      </c>
+      <c r="B248" s="5">
+        <v>6</v>
+      </c>
+      <c r="C248" s="5">
+        <v>1</v>
+      </c>
+      <c r="D248" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E248" s="5">
+        <v>1</v>
+      </c>
+      <c r="F248" s="5">
+        <v>48014</v>
+      </c>
+      <c r="G248" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H248" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A249" s="5">
+        <v>62</v>
+      </c>
+      <c r="B249" s="5">
+        <v>7</v>
+      </c>
+      <c r="C249" s="5">
+        <v>1</v>
+      </c>
+      <c r="D249" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" s="5">
+        <v>1</v>
+      </c>
+      <c r="F249" s="5">
+        <v>20465</v>
+      </c>
+      <c r="G249" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H249" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250" s="5">
+        <v>62</v>
+      </c>
+      <c r="B250" s="5">
+        <v>8</v>
+      </c>
+      <c r="C250" s="5">
+        <v>1</v>
+      </c>
+      <c r="D250" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250" s="5">
+        <v>0</v>
+      </c>
+      <c r="F250" s="5">
+        <v>45549</v>
+      </c>
+      <c r="G250" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H250" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A251" s="5">
+        <v>62</v>
+      </c>
+      <c r="B251" s="5">
+        <v>9</v>
+      </c>
+      <c r="C251" s="5">
+        <v>1</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E251" s="5">
+        <v>0</v>
+      </c>
+      <c r="F251" s="5">
+        <v>36964</v>
+      </c>
+      <c r="G251" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H251" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A252" s="5">
+        <v>62</v>
+      </c>
+      <c r="B252" s="5">
+        <v>10</v>
+      </c>
+      <c r="C252" s="5">
+        <v>1</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E252" s="5">
+        <v>0</v>
+      </c>
+      <c r="F252" s="5">
+        <v>36076</v>
+      </c>
+      <c r="G252" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H252" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A253" s="5">
+        <v>62</v>
+      </c>
+      <c r="B253" s="5">
+        <v>11</v>
+      </c>
+      <c r="C253" s="5">
+        <v>1</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E253" s="5">
+        <v>0</v>
+      </c>
+      <c r="F253" s="5">
+        <v>52299</v>
+      </c>
+      <c r="G253" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H253" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A254" s="5">
+        <v>62</v>
+      </c>
+      <c r="B254" s="5">
+        <v>12</v>
+      </c>
+      <c r="C254" s="5">
+        <v>1</v>
+      </c>
+      <c r="D254" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E254" s="5">
+        <v>1</v>
+      </c>
+      <c r="F254" s="5">
+        <v>41556</v>
+      </c>
+      <c r="G254" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H254" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A255" s="5">
+        <v>62</v>
+      </c>
+      <c r="B255" s="5">
+        <v>13</v>
+      </c>
+      <c r="C255" s="5">
+        <v>1</v>
+      </c>
+      <c r="D255" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E255" s="5">
+        <v>1</v>
+      </c>
+      <c r="F255" s="5">
+        <v>62475</v>
+      </c>
+      <c r="G255" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H255" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A256" s="5">
+        <v>62</v>
+      </c>
+      <c r="B256" s="5">
+        <v>14</v>
+      </c>
+      <c r="C256" s="5">
+        <v>1</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E256" s="5">
+        <v>1</v>
+      </c>
+      <c r="F256" s="5">
+        <v>29771</v>
+      </c>
+      <c r="G256" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H256" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A257" s="5">
+        <v>62</v>
+      </c>
+      <c r="B257" s="5">
+        <v>15</v>
+      </c>
+      <c r="C257" s="5">
+        <v>1</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E257" s="5">
+        <v>1</v>
+      </c>
+      <c r="F257" s="5">
+        <v>13116</v>
+      </c>
+      <c r="G257" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H257" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A258" s="5">
+        <v>62</v>
+      </c>
+      <c r="B258" s="5">
+        <v>16</v>
+      </c>
+      <c r="C258" s="5">
+        <v>0</v>
+      </c>
+      <c r="D258" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E258" s="5">
+        <v>0</v>
+      </c>
+      <c r="F258" s="5">
+        <v>64884</v>
+      </c>
+      <c r="G258" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H258" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A259" s="5">
+        <v>62</v>
+      </c>
+      <c r="B259" s="5">
+        <v>17</v>
+      </c>
+      <c r="C259" s="5">
+        <v>0</v>
+      </c>
+      <c r="D259" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" s="5">
+        <v>0</v>
+      </c>
+      <c r="F259" s="5">
+        <v>30708</v>
+      </c>
+      <c r="G259" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H259" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A260" s="5">
+        <v>62</v>
+      </c>
+      <c r="B260" s="5">
+        <v>18</v>
+      </c>
+      <c r="C260" s="5">
+        <v>0</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E260" s="5">
+        <v>0</v>
+      </c>
+      <c r="F260" s="5">
+        <v>72603</v>
+      </c>
+      <c r="G260" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H260" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A261" s="5">
+        <v>62</v>
+      </c>
+      <c r="B261" s="5">
+        <v>19</v>
+      </c>
+      <c r="C261" s="5">
+        <v>0</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E261" s="5">
+        <v>0</v>
+      </c>
+      <c r="F261" s="5">
+        <v>26956</v>
+      </c>
+      <c r="G261" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H261" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A262" s="5">
+        <v>62</v>
+      </c>
+      <c r="B262" s="5">
+        <v>20</v>
+      </c>
+      <c r="C262" s="5">
+        <v>0</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262" s="5">
+        <v>1</v>
+      </c>
+      <c r="F262" s="5">
+        <v>24460</v>
+      </c>
+      <c r="G262" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H262" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A263" s="5">
+        <v>62</v>
+      </c>
+      <c r="B263" s="5">
+        <v>21</v>
+      </c>
+      <c r="C263" s="5">
+        <v>0</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E263" s="5">
+        <v>1</v>
+      </c>
+      <c r="F263" s="5">
+        <v>28516</v>
+      </c>
+      <c r="G263" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H263" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A264" s="5">
+        <v>62</v>
+      </c>
+      <c r="B264" s="5">
+        <v>22</v>
+      </c>
+      <c r="C264" s="5">
+        <v>0</v>
+      </c>
+      <c r="D264" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E264" s="5">
+        <v>1</v>
+      </c>
+      <c r="F264" s="5">
+        <v>41996</v>
+      </c>
+      <c r="G264" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H264" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A265" s="5">
+        <v>62</v>
+      </c>
+      <c r="B265" s="5">
+        <v>23</v>
+      </c>
+      <c r="C265" s="5">
+        <v>0</v>
+      </c>
+      <c r="D265" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E265" s="5">
+        <v>1</v>
+      </c>
+      <c r="F265" s="5">
+        <v>18804</v>
+      </c>
+      <c r="G265" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H265" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A266" s="5">
+        <v>62</v>
+      </c>
+      <c r="B266" s="5">
+        <v>24</v>
+      </c>
+      <c r="C266" s="5">
+        <v>0</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E266" s="5">
+        <v>0</v>
+      </c>
+      <c r="F266" s="5">
+        <v>13833</v>
+      </c>
+      <c r="G266" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H266" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A267" s="5">
+        <v>62</v>
+      </c>
+      <c r="B267" s="5">
+        <v>25</v>
+      </c>
+      <c r="C267" s="5">
+        <v>0</v>
+      </c>
+      <c r="D267" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E267" s="5">
+        <v>0</v>
+      </c>
+      <c r="F267" s="5">
+        <v>15249</v>
+      </c>
+      <c r="G267" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H267" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A268" s="5">
+        <v>62</v>
+      </c>
+      <c r="B268" s="5">
+        <v>26</v>
+      </c>
+      <c r="C268" s="5">
+        <v>0</v>
+      </c>
+      <c r="D268" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E268" s="5">
+        <v>0</v>
+      </c>
+      <c r="F268" s="5">
+        <v>19648</v>
+      </c>
+      <c r="G268" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H268" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A269" s="5">
+        <v>62</v>
+      </c>
+      <c r="B269" s="5">
+        <v>27</v>
+      </c>
+      <c r="C269" s="5">
+        <v>0</v>
+      </c>
+      <c r="D269" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E269" s="5">
+        <v>0</v>
+      </c>
+      <c r="F269" s="5">
+        <v>17496</v>
+      </c>
+      <c r="G269" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H269" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A270" s="5">
+        <v>62</v>
+      </c>
+      <c r="B270" s="5">
+        <v>28</v>
+      </c>
+      <c r="C270" s="5">
+        <v>0</v>
+      </c>
+      <c r="D270" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E270" s="5">
+        <v>1</v>
+      </c>
+      <c r="F270" s="5">
+        <v>49431</v>
+      </c>
+      <c r="G270" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H270" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A271" s="5">
+        <v>62</v>
+      </c>
+      <c r="B271" s="5">
+        <v>29</v>
+      </c>
+      <c r="C271" s="5">
+        <v>0</v>
+      </c>
+      <c r="D271" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" s="5">
+        <v>1</v>
+      </c>
+      <c r="F271" s="5">
+        <v>23080</v>
+      </c>
+      <c r="G271" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H271" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A272" s="5">
+        <v>62</v>
+      </c>
+      <c r="B272" s="5">
+        <v>30</v>
+      </c>
+      <c r="C272" s="5">
+        <v>0</v>
+      </c>
+      <c r="D272" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E272" s="5">
+        <v>1</v>
+      </c>
+      <c r="F272" s="5">
+        <v>42384</v>
+      </c>
+      <c r="G272" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H272" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A273" s="5">
+        <v>62</v>
+      </c>
+      <c r="B273" s="5">
+        <v>31</v>
+      </c>
+      <c r="C273" s="5">
+        <v>0</v>
+      </c>
+      <c r="D273" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E273" s="5">
+        <v>1</v>
+      </c>
+      <c r="F273" s="5">
+        <v>14546</v>
+      </c>
+      <c r="G273" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H273" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" s="5">
+        <v>62</v>
+      </c>
+      <c r="B274" s="5">
+        <v>32</v>
+      </c>
+      <c r="C274" s="5">
+        <v>2</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E274" s="5">
+        <v>0</v>
+      </c>
+      <c r="F274" s="5">
+        <v>24442</v>
+      </c>
+      <c r="G274" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H274" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" s="5">
+        <v>62</v>
+      </c>
+      <c r="B275" s="5">
+        <v>33</v>
+      </c>
+      <c r="C275" s="5">
+        <v>2</v>
+      </c>
+      <c r="D275" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E275" s="5">
+        <v>0</v>
+      </c>
+      <c r="F275" s="5">
+        <v>17768</v>
+      </c>
+      <c r="G275" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H275" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A276" s="5">
+        <v>62</v>
+      </c>
+      <c r="B276" s="5">
+        <v>34</v>
+      </c>
+      <c r="C276" s="5">
+        <v>2</v>
+      </c>
+      <c r="D276" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E276" s="5">
+        <v>0</v>
+      </c>
+      <c r="F276" s="5">
+        <v>12146</v>
+      </c>
+      <c r="G276" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H276" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A277" s="5">
+        <v>62</v>
+      </c>
+      <c r="B277" s="5">
+        <v>35</v>
+      </c>
+      <c r="C277" s="5">
+        <v>2</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E277" s="5">
+        <v>0</v>
+      </c>
+      <c r="F277" s="5">
+        <v>16025</v>
+      </c>
+      <c r="G277" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H277" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A278" s="5">
+        <v>62</v>
+      </c>
+      <c r="B278" s="5">
+        <v>36</v>
+      </c>
+      <c r="C278" s="5">
+        <v>2</v>
+      </c>
+      <c r="D278" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E278" s="5">
+        <v>1</v>
+      </c>
+      <c r="F278" s="5">
+        <v>20368</v>
+      </c>
+      <c r="G278" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H278" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A279" s="5">
+        <v>62</v>
+      </c>
+      <c r="B279" s="5">
+        <v>37</v>
+      </c>
+      <c r="C279" s="5">
+        <v>2</v>
+      </c>
+      <c r="D279" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E279" s="5">
+        <v>1</v>
+      </c>
+      <c r="F279" s="5">
+        <v>36848</v>
+      </c>
+      <c r="G279" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H279" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A280" s="5">
+        <v>62</v>
+      </c>
+      <c r="B280" s="5">
+        <v>38</v>
+      </c>
+      <c r="C280" s="5">
+        <v>2</v>
+      </c>
+      <c r="D280" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E280" s="5">
+        <v>1</v>
+      </c>
+      <c r="F280" s="5">
+        <v>11824</v>
+      </c>
+      <c r="G280" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H280" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A281" s="5">
+        <v>62</v>
+      </c>
+      <c r="B281" s="5">
+        <v>39</v>
+      </c>
+      <c r="C281" s="5">
+        <v>2</v>
+      </c>
+      <c r="D281" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E281" s="5">
+        <v>1</v>
+      </c>
+      <c r="F281" s="5">
+        <v>33720</v>
+      </c>
+      <c r="G281" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H281" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A282" s="5">
+        <v>62</v>
+      </c>
+      <c r="B282" s="5">
+        <v>40</v>
+      </c>
+      <c r="C282" s="5">
+        <v>2</v>
+      </c>
+      <c r="D282" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E282" s="5">
+        <v>0</v>
+      </c>
+      <c r="F282" s="5">
+        <v>24315</v>
+      </c>
+      <c r="G282" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H282" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A283" s="5">
+        <v>62</v>
+      </c>
+      <c r="B283" s="5">
+        <v>41</v>
+      </c>
+      <c r="C283" s="5">
+        <v>2</v>
+      </c>
+      <c r="D283" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E283" s="5">
+        <v>0</v>
+      </c>
+      <c r="F283" s="5">
+        <v>38795</v>
+      </c>
+      <c r="G283" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H283" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A284" s="5">
+        <v>62</v>
+      </c>
+      <c r="B284" s="5">
+        <v>42</v>
+      </c>
+      <c r="C284" s="5">
+        <v>2</v>
+      </c>
+      <c r="D284" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E284" s="5">
+        <v>0</v>
+      </c>
+      <c r="F284" s="5">
+        <v>25155</v>
+      </c>
+      <c r="G284" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H284" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A285" s="5">
+        <v>62</v>
+      </c>
+      <c r="B285" s="5">
+        <v>43</v>
+      </c>
+      <c r="C285" s="5">
+        <v>2</v>
+      </c>
+      <c r="D285" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E285" s="5">
+        <v>0</v>
+      </c>
+      <c r="F285" s="5">
+        <v>11564</v>
+      </c>
+      <c r="G285" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H285" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A286" s="5">
+        <v>62</v>
+      </c>
+      <c r="B286" s="5">
+        <v>44</v>
+      </c>
+      <c r="C286" s="5">
+        <v>2</v>
+      </c>
+      <c r="D286" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E286" s="5">
+        <v>1</v>
+      </c>
+      <c r="F286" s="5">
+        <v>7996</v>
+      </c>
+      <c r="G286" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H286" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A287" s="5">
+        <v>62</v>
+      </c>
+      <c r="B287" s="5">
+        <v>45</v>
+      </c>
+      <c r="C287" s="5">
+        <v>2</v>
+      </c>
+      <c r="D287" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E287" s="5">
+        <v>1</v>
+      </c>
+      <c r="F287" s="5">
+        <v>17876</v>
+      </c>
+      <c r="G287" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H287" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A288" s="5">
+        <v>62</v>
+      </c>
+      <c r="B288" s="5">
+        <v>46</v>
+      </c>
+      <c r="C288" s="5">
+        <v>2</v>
+      </c>
+      <c r="D288" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E288" s="5">
+        <v>1</v>
+      </c>
+      <c r="F288" s="5">
+        <v>22764</v>
+      </c>
+      <c r="G288" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H288" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A289" s="5">
+        <v>62</v>
+      </c>
+      <c r="B289" s="5">
+        <v>47</v>
+      </c>
+      <c r="C289" s="5">
+        <v>2</v>
+      </c>
+      <c r="D289" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E289" s="5">
+        <v>1</v>
+      </c>
+      <c r="F289" s="5">
+        <v>21211</v>
+      </c>
+      <c r="G289" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H289" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>